<commit_message>
7RSUPERMARKET NEW CHANGES _Assertion
</commit_message>
<xml_diff>
--- a/7RMartSuperMarketProject/src/test/resources/TestData.xlsx
+++ b/7RMartSuperMarketProject/src/test/resources/TestData.xlsx
@@ -1,16 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28827"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hp\git\AutoRepo\AutomationRepo\7RMartSuperMarketProject\src\test\resources\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2BB8E16-AFFE-4567-9C1F-908B334D19BB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{9B3C63C4-F8C3-4855-96AE-30B7FDAE3CC3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="LoginPage" sheetId="1" r:id="rId1"/>
@@ -19,6 +14,7 @@
     <sheet name="ManageCategoryPage" sheetId="5" r:id="rId4"/>
   </sheets>
   <calcPr calcId="0"/>
+  <oleSize ref="A1:N3"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -365,7 +361,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
@@ -456,7 +452,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A8471B7D-443F-44E6-B91B-4DEB698442A0}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>

</xml_diff>